<commit_message>
Was missing an efficiency! Now fixed.
</commit_message>
<xml_diff>
--- a/inst/extdata/GH-ZA-Efficiency-sample-2019.xlsx
+++ b/inst/extdata/GH-ZA-Efficiency-sample-2019.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/github/IEATools/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{574C44D9-6F11-0649-AAA6-F2E425B00E61}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9069BD6-1DA2-3B42-932B-45BB1DC8445F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28180" yWindow="460" windowWidth="22820" windowHeight="28340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -620,8 +620,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K305"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="F100" sqref="F100"/>
+    <sheetView tabSelected="1" topLeftCell="A227" workbookViewId="0">
+      <selection activeCell="J268" sqref="J268:K268"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9590,7 +9590,9 @@
       <c r="J268" s="4">
         <v>0.85</v>
       </c>
-      <c r="K268" s="4"/>
+      <c r="K268" s="4">
+        <v>0.85</v>
+      </c>
     </row>
     <row r="269" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A269" s="5" t="s">

</xml_diff>

<commit_message>
Tests for eta_fu_table_completed are done.
</commit_message>
<xml_diff>
--- a/inst/extdata/GH-ZA-Efficiency-sample-2019.xlsx
+++ b/inst/extdata/GH-ZA-Efficiency-sample-2019.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/github/IEATools/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9069BD6-1DA2-3B42-932B-45BB1DC8445F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6141221-0543-F043-B0C3-940D381FB908}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28180" yWindow="460" windowWidth="22820" windowHeight="28340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,19 +16,11 @@
     <sheet name="FU etas" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2443" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2443" uniqueCount="69">
   <si>
     <t>Country</t>
   </si>
@@ -211,9 +203,6 @@
   </si>
   <si>
     <t>Wood furnaces</t>
-  </si>
-  <si>
-    <t>Non-energy use industry/transformation/energy</t>
   </si>
   <si>
     <t>Bitumen</t>
@@ -620,8 +609,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K305"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A227" workbookViewId="0">
-      <selection activeCell="J268" sqref="J268:K268"/>
+    <sheetView tabSelected="1" topLeftCell="A248" workbookViewId="0">
+      <selection activeCell="F315" sqref="F315"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3658,10 +3647,10 @@
         <v>15</v>
       </c>
       <c r="F90" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G90" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H90" s="2" t="s">
         <v>18</v>
@@ -3691,10 +3680,10 @@
         <v>15</v>
       </c>
       <c r="F91" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G91" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H91" s="2" t="s">
         <v>19</v>
@@ -3724,10 +3713,10 @@
         <v>15</v>
       </c>
       <c r="F92" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G92" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H92" s="5" t="s">
         <v>20</v>
@@ -3755,10 +3744,10 @@
         <v>15</v>
       </c>
       <c r="F93" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G93" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H93" s="5" t="s">
         <v>21</v>
@@ -3786,10 +3775,10 @@
         <v>15</v>
       </c>
       <c r="F94" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G94" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H94" s="2" t="s">
         <v>18</v>
@@ -3821,10 +3810,10 @@
         <v>15</v>
       </c>
       <c r="F95" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G95" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H95" s="2" t="s">
         <v>19</v>
@@ -3856,10 +3845,10 @@
         <v>15</v>
       </c>
       <c r="F96" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G96" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H96" s="5" t="s">
         <v>20</v>
@@ -3889,10 +3878,10 @@
         <v>15</v>
       </c>
       <c r="F97" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G97" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H97" s="5" t="s">
         <v>21</v>
@@ -3922,10 +3911,10 @@
         <v>15</v>
       </c>
       <c r="F98" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G98" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H98" s="2" t="s">
         <v>18</v>
@@ -3955,10 +3944,10 @@
         <v>15</v>
       </c>
       <c r="F99" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G99" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H99" s="2" t="s">
         <v>19</v>
@@ -3988,10 +3977,10 @@
         <v>15</v>
       </c>
       <c r="F100" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G100" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H100" s="5" t="s">
         <v>20</v>
@@ -4019,10 +4008,10 @@
         <v>15</v>
       </c>
       <c r="F101" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G101" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H101" s="5" t="s">
         <v>21</v>
@@ -10028,10 +10017,10 @@
         <v>15</v>
       </c>
       <c r="F282" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="G282" s="2" t="s">
         <v>61</v>
-      </c>
-      <c r="G282" s="2" t="s">
-        <v>62</v>
       </c>
       <c r="H282" s="2" t="s">
         <v>18</v>
@@ -10063,10 +10052,10 @@
         <v>15</v>
       </c>
       <c r="F283" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="G283" s="2" t="s">
         <v>61</v>
-      </c>
-      <c r="G283" s="2" t="s">
-        <v>62</v>
       </c>
       <c r="H283" s="2" t="s">
         <v>19</v>
@@ -10098,10 +10087,10 @@
         <v>15</v>
       </c>
       <c r="F284" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="G284" s="5" t="s">
         <v>61</v>
-      </c>
-      <c r="G284" s="5" t="s">
-        <v>62</v>
       </c>
       <c r="H284" s="5" t="s">
         <v>20</v>
@@ -10131,10 +10120,10 @@
         <v>15</v>
       </c>
       <c r="F285" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="G285" s="5" t="s">
         <v>61</v>
-      </c>
-      <c r="G285" s="5" t="s">
-        <v>62</v>
       </c>
       <c r="H285" s="5" t="s">
         <v>21</v>
@@ -10164,10 +10153,10 @@
         <v>15</v>
       </c>
       <c r="F286" s="2" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="G286" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H286" s="2" t="s">
         <v>18</v>
@@ -10197,10 +10186,10 @@
         <v>15</v>
       </c>
       <c r="F287" s="2" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="G287" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H287" s="2" t="s">
         <v>19</v>
@@ -10230,10 +10219,10 @@
         <v>15</v>
       </c>
       <c r="F288" s="5" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="G288" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H288" s="5" t="s">
         <v>20</v>
@@ -10261,10 +10250,10 @@
         <v>15</v>
       </c>
       <c r="F289" s="5" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="G289" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H289" s="5" t="s">
         <v>21</v>
@@ -10292,10 +10281,10 @@
         <v>15</v>
       </c>
       <c r="F290" s="2" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="G290" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H290" s="2" t="s">
         <v>18</v>
@@ -10325,10 +10314,10 @@
         <v>15</v>
       </c>
       <c r="F291" s="2" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="G291" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H291" s="2" t="s">
         <v>19</v>
@@ -10358,10 +10347,10 @@
         <v>15</v>
       </c>
       <c r="F292" s="5" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="G292" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H292" s="5" t="s">
         <v>20</v>
@@ -10389,10 +10378,10 @@
         <v>15</v>
       </c>
       <c r="F293" s="5" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="G293" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H293" s="5" t="s">
         <v>21</v>
@@ -10420,10 +10409,10 @@
         <v>15</v>
       </c>
       <c r="F294" s="2" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="G294" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H294" s="2" t="s">
         <v>18</v>
@@ -10453,10 +10442,10 @@
         <v>15</v>
       </c>
       <c r="F295" s="2" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="G295" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H295" s="2" t="s">
         <v>19</v>
@@ -10486,10 +10475,10 @@
         <v>15</v>
       </c>
       <c r="F296" s="5" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="G296" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H296" s="5" t="s">
         <v>20</v>
@@ -10517,10 +10506,10 @@
         <v>15</v>
       </c>
       <c r="F297" s="5" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="G297" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H297" s="5" t="s">
         <v>21</v>
@@ -10548,10 +10537,10 @@
         <v>15</v>
       </c>
       <c r="F298" s="2" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="G298" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H298" s="2" t="s">
         <v>18</v>
@@ -10581,10 +10570,10 @@
         <v>15</v>
       </c>
       <c r="F299" s="2" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="G299" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H299" s="2" t="s">
         <v>19</v>
@@ -10614,10 +10603,10 @@
         <v>15</v>
       </c>
       <c r="F300" s="5" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="G300" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H300" s="5" t="s">
         <v>20</v>
@@ -10645,10 +10634,10 @@
         <v>15</v>
       </c>
       <c r="F301" s="5" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="G301" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H301" s="5" t="s">
         <v>21</v>
@@ -10676,10 +10665,10 @@
         <v>15</v>
       </c>
       <c r="F302" s="2" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="G302" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H302" s="2" t="s">
         <v>18</v>
@@ -10709,10 +10698,10 @@
         <v>15</v>
       </c>
       <c r="F303" s="2" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="G303" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H303" s="2" t="s">
         <v>19</v>
@@ -10742,10 +10731,10 @@
         <v>15</v>
       </c>
       <c r="F304" s="5" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="G304" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H304" s="5" t="s">
         <v>20</v>
@@ -10773,10 +10762,10 @@
         <v>15</v>
       </c>
       <c r="F305" s="5" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="G305" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H305" s="5" t="s">
         <v>21</v>

</xml_diff>

<commit_message>
Wood stoves --> Wood cookstoves to be consistent.
</commit_message>
<xml_diff>
--- a/inst/extdata/GH-ZA-Efficiency-sample-2019.xlsx
+++ b/inst/extdata/GH-ZA-Efficiency-sample-2019.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/github/IEATools/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6141221-0543-F043-B0C3-940D381FB908}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E603C71-0898-6047-9F49-5CF1C4B5AE6B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28180" yWindow="460" windowWidth="22820" windowHeight="28340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -609,8 +609,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K305"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A248" workbookViewId="0">
-      <selection activeCell="F315" sqref="F315"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="F70" sqref="F70:F73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2967,7 +2967,7 @@
         <v>15</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>34</v>
+        <v>57</v>
       </c>
       <c r="G70" s="2" t="s">
         <v>39</v>
@@ -3002,7 +3002,7 @@
         <v>15</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>34</v>
+        <v>57</v>
       </c>
       <c r="G71" s="2" t="s">
         <v>39</v>
@@ -3037,7 +3037,7 @@
         <v>15</v>
       </c>
       <c r="F72" s="5" t="s">
-        <v>34</v>
+        <v>57</v>
       </c>
       <c r="G72" s="5" t="s">
         <v>39</v>
@@ -3070,7 +3070,7 @@
         <v>15</v>
       </c>
       <c r="F73" s="5" t="s">
-        <v>34</v>
+        <v>57</v>
       </c>
       <c r="G73" s="5" t="s">
         <v>39</v>

</xml_diff>